<commit_message>
Added Component References to Register BOM
</commit_message>
<xml_diff>
--- a/register/BOM.xlsx
+++ b/register/BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
   <si>
     <t>ULN2803A</t>
   </si>
@@ -123,6 +123,27 @@
   </si>
   <si>
     <t xml:space="preserve">DILB18P223TLF </t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>R1..8</t>
+  </si>
+  <si>
+    <t>D1..8</t>
+  </si>
+  <si>
+    <t>U2, U5</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>C1..3</t>
   </si>
 </sst>
 </file>
@@ -458,7 +479,7 @@
   <dimension ref="B1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,16 +515,22 @@
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>27</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
@@ -519,6 +546,9 @@
       <c r="F3">
         <v>8</v>
       </c>
+      <c r="G3" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -536,6 +566,9 @@
       <c r="F4">
         <v>8</v>
       </c>
+      <c r="G4" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
@@ -550,50 +583,59 @@
       <c r="F5">
         <v>1</v>
       </c>
+      <c r="G5" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>22</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="G6" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="F7">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F8">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
@@ -601,13 +643,16 @@
         <v>28</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F9">
         <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
@@ -615,13 +660,16 @@
         <v>28</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="G10" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
@@ -629,13 +677,16 @@
         <v>28</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F11">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
@@ -643,16 +694,22 @@
         <v>28</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F12">
         <v>1</v>
       </c>
+      <c r="G12" t="s">
+        <v>37</v>
+      </c>
     </row>
   </sheetData>
+  <sortState ref="B9:G12">
+    <sortCondition ref="G12"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>